<commit_message>
genesis correjido y listo
</commit_message>
<xml_diff>
--- a/Proyectos Evaluados/Genesis/Antecedentes PF - Génesis_V2 - Resultados TIR.xlsx
+++ b/Proyectos Evaluados/Genesis/Antecedentes PF - Génesis_V2 - Resultados TIR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephano Chaura\Desktop\ejecucion-modelos\Proyectos Evaluados\Genesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A5D75F-97DA-4E84-A360-15E0A72E833F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E5F4D8-5FD1-4765-8361-CB1002CC607D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{A8E2847A-B53C-4F40-AC56-E093DD92F3C8}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{A8E2847A-B53C-4F40-AC56-E093DD92F3C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Caso PMG" sheetId="1" r:id="rId1"/>
@@ -896,7 +896,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1126,6 +1126,15 @@
     <xf numFmtId="10" fontId="5" fillId="7" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="3" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1169,15 +1178,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="10" fontId="5" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="3" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1542,12 +1542,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1564,7 +1564,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="34" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1578,7 +1578,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1590,7 +1590,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="2" t="s">
         <v>43</v>
       </c>
@@ -1602,7 +1602,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1614,7 +1614,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="33" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1628,7 +1628,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1640,7 +1640,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
@@ -1666,7 +1666,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1680,7 +1680,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1692,7 +1692,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="3" t="s">
         <v>28</v>
       </c>
@@ -1704,7 +1704,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
@@ -1716,7 +1716,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="35" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1730,7 +1730,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1742,7 +1742,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1754,7 +1754,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1766,7 +1766,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1778,7 +1778,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="2" t="s">
         <v>25</v>
       </c>
@@ -1790,7 +1790,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="2" t="s">
         <v>26</v>
       </c>
@@ -1802,7 +1802,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1828,7 +1828,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="3" t="s">
         <v>30</v>
       </c>
@@ -1841,7 +1841,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="3" t="s">
         <v>31</v>
       </c>
@@ -1869,7 +1869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8A343BC-6ED4-4CBF-9CE7-6A372F00A3DD}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -1882,12 +1882,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1904,7 +1904,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="34" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1918,7 +1918,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1930,7 +1930,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="2" t="s">
         <v>43</v>
       </c>
@@ -1942,7 +1942,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1954,7 +1954,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="33" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1968,7 +1968,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1980,7 +1980,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
@@ -2006,7 +2006,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2020,7 +2020,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
@@ -2032,7 +2032,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="3" t="s">
         <v>28</v>
       </c>
@@ -2044,7 +2044,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
@@ -2056,7 +2056,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="35" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -2070,7 +2070,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
@@ -2082,7 +2082,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="2" t="s">
         <v>21</v>
       </c>
@@ -2094,7 +2094,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
@@ -2106,7 +2106,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
@@ -2118,7 +2118,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="2" t="s">
         <v>25</v>
       </c>
@@ -2130,7 +2130,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="2" t="s">
         <v>26</v>
       </c>
@@ -2142,7 +2142,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="2" t="s">
         <v>27</v>
       </c>
@@ -2154,7 +2154,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="29" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -2168,7 +2168,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="3" t="s">
         <v>30</v>
       </c>
@@ -2181,7 +2181,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="3" t="s">
         <v>31</v>
       </c>
@@ -72322,8 +72322,8 @@
   </sheetPr>
   <dimension ref="B2:G39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C12" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72517,37 +72517,37 @@
       <c r="B12" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="37"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="40"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="40"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="43"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="40"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
@@ -72561,61 +72561,61 @@
       <c r="B16" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="40"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="40"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="43"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="37"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="40"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="40"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="43"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="37"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="40"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
@@ -72640,16 +72640,16 @@
         <v>72</v>
       </c>
       <c r="C23" s="24">
-        <v>7.5899999999999995E-2</v>
+        <v>7.3599999999999999E-2</v>
       </c>
       <c r="D23" s="24">
-        <v>8.4000000000000005E-2</v>
+        <v>8.1900000000000001E-2</v>
       </c>
       <c r="E23" s="13">
-        <v>1.17</v>
+        <v>0.99</v>
       </c>
       <c r="F23" s="13">
-        <v>9.3000000000000007</v>
+        <v>9.4</v>
       </c>
       <c r="G23" s="13">
         <v>58.5</v>
@@ -72660,16 +72660,16 @@
         <v>73</v>
       </c>
       <c r="C24" s="25">
-        <v>8.2000000000000003E-2</v>
+        <v>7.7600000000000002E-2</v>
       </c>
       <c r="D24" s="25">
-        <v>8.9599999999999999E-2</v>
+        <v>8.5400000000000004E-2</v>
       </c>
       <c r="E24" s="15">
-        <v>1.82</v>
+        <v>1.42</v>
       </c>
       <c r="F24" s="15">
-        <v>8.8000000000000007</v>
+        <v>9</v>
       </c>
       <c r="G24" s="15">
         <v>65.599999999999994</v>
@@ -72680,16 +72680,16 @@
         <v>74</v>
       </c>
       <c r="C25" s="45">
-        <v>8.2299999999999998E-2</v>
+        <v>7.6200000000000004E-2</v>
       </c>
       <c r="D25" s="45">
-        <v>8.9899999999999994E-2</v>
+        <v>8.4099999999999994E-2</v>
       </c>
       <c r="E25" s="46">
-        <v>2.02</v>
+        <v>1.41</v>
       </c>
       <c r="F25" s="46">
-        <v>8.6999999999999993</v>
+        <v>9</v>
       </c>
       <c r="G25" s="46">
         <v>72.8</v>
@@ -72700,16 +72700,16 @@
         <v>75</v>
       </c>
       <c r="C26" s="25">
-        <v>7.6100000000000001E-2</v>
+        <v>6.8400000000000002E-2</v>
       </c>
       <c r="D26" s="25">
-        <v>8.43E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="E26" s="15">
-        <v>1.58</v>
+        <v>0.76</v>
       </c>
       <c r="F26" s="15">
-        <v>9</v>
+        <v>9.4</v>
       </c>
       <c r="G26" s="15">
         <v>80</v>
@@ -72720,16 +72720,16 @@
         <v>76</v>
       </c>
       <c r="C27" s="24">
-        <v>6.8400000000000002E-2</v>
+        <v>5.9299999999999999E-2</v>
       </c>
       <c r="D27" s="24">
-        <v>7.7399999999999997E-2</v>
+        <v>6.88E-2</v>
       </c>
       <c r="E27" s="13">
-        <v>0.87</v>
+        <v>-0.13</v>
       </c>
       <c r="F27" s="13">
-        <v>9.5</v>
+        <v>11.7</v>
       </c>
       <c r="G27" s="13">
         <v>87.3</v>
@@ -72748,16 +72748,16 @@
         <v>67</v>
       </c>
       <c r="C29" s="24">
-        <v>7.46E-2</v>
+        <v>7.2800000000000004E-2</v>
       </c>
       <c r="D29" s="24">
-        <v>8.2900000000000001E-2</v>
+        <v>8.1199999999999994E-2</v>
       </c>
       <c r="E29" s="13">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="F29" s="13">
-        <v>9.4</v>
+        <v>9.5</v>
       </c>
       <c r="G29" s="13">
         <v>56</v>
@@ -72768,39 +72768,39 @@
         <v>68</v>
       </c>
       <c r="C30" s="25">
-        <v>8.09E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="D30" s="25">
-        <v>8.8599999999999998E-2</v>
+        <v>8.4900000000000003E-2</v>
       </c>
       <c r="E30" s="15">
-        <v>1.83</v>
+        <v>1.45</v>
       </c>
       <c r="F30" s="15">
-        <v>8.9</v>
+        <v>9.1</v>
       </c>
       <c r="G30" s="15">
         <v>62.4</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="42">
-        <v>8.1799999999999998E-2</v>
-      </c>
-      <c r="D31" s="42">
-        <v>8.9499999999999996E-2</v>
-      </c>
-      <c r="E31" s="43">
-        <v>2.09</v>
-      </c>
-      <c r="F31" s="43">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="G31" s="43">
-        <v>68.900000000000006</v>
+      <c r="C31" s="27">
+        <v>7.6100000000000001E-2</v>
+      </c>
+      <c r="D31" s="27">
+        <v>8.4099999999999994E-2</v>
+      </c>
+      <c r="E31" s="28">
+        <v>1.49</v>
+      </c>
+      <c r="F31" s="28">
+        <v>9</v>
+      </c>
+      <c r="G31" s="28">
+        <v>68.8</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
@@ -72808,16 +72808,16 @@
         <v>70</v>
       </c>
       <c r="C32" s="25">
-        <v>7.6600000000000001E-2</v>
+        <v>6.93E-2</v>
       </c>
       <c r="D32" s="25">
-        <v>8.4900000000000003E-2</v>
+        <v>7.7899999999999997E-2</v>
       </c>
       <c r="E32" s="15">
-        <v>1.72</v>
+        <v>0.91</v>
       </c>
       <c r="F32" s="15">
-        <v>9</v>
+        <v>9.4</v>
       </c>
       <c r="G32" s="15">
         <v>75.400000000000006</v>
@@ -72828,16 +72828,16 @@
         <v>71</v>
       </c>
       <c r="C33" s="24">
-        <v>6.9900000000000004E-2</v>
+        <v>6.1100000000000002E-2</v>
       </c>
       <c r="D33" s="24">
-        <v>7.8799999999999995E-2</v>
+        <v>7.0599999999999996E-2</v>
       </c>
       <c r="E33" s="13">
-        <v>1.1000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F33" s="13">
-        <v>9.4</v>
+        <v>10.1</v>
       </c>
       <c r="G33" s="13">
         <v>81.900000000000006</v>
@@ -72856,16 +72856,16 @@
         <v>79</v>
       </c>
       <c r="C35" s="24">
-        <v>7.3200000000000001E-2</v>
+        <v>7.1900000000000006E-2</v>
       </c>
       <c r="D35" s="24">
-        <v>8.1600000000000006E-2</v>
+        <v>8.0399999999999999E-2</v>
       </c>
       <c r="E35" s="13">
-        <v>1.1000000000000001</v>
+        <v>0.98</v>
       </c>
       <c r="F35" s="13">
-        <v>9.5</v>
+        <v>9.6</v>
       </c>
       <c r="G35" s="13">
         <v>54</v>
@@ -72876,38 +72876,38 @@
         <v>77</v>
       </c>
       <c r="C36" s="25">
-        <v>7.9600000000000004E-2</v>
+        <v>7.6100000000000001E-2</v>
       </c>
       <c r="D36" s="25">
-        <v>8.7499999999999994E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
       <c r="E36" s="15">
-        <v>1.81</v>
+        <v>1.46</v>
       </c>
       <c r="F36" s="15">
-        <v>8.98</v>
+        <v>9.17</v>
       </c>
       <c r="G36" s="15">
         <v>59.8</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="42">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="D37" s="42">
-        <v>8.8800000000000004E-2</v>
-      </c>
-      <c r="E37" s="43">
-        <v>2.12</v>
-      </c>
-      <c r="F37" s="43">
-        <v>8.83</v>
-      </c>
-      <c r="G37" s="43">
+      <c r="C37" s="27">
+        <v>7.5700000000000003E-2</v>
+      </c>
+      <c r="D37" s="27">
+        <v>8.2799999999999999E-2</v>
+      </c>
+      <c r="E37" s="28">
+        <v>1.54</v>
+      </c>
+      <c r="F37" s="28">
+        <v>9.1</v>
+      </c>
+      <c r="G37" s="28">
         <v>65.7</v>
       </c>
     </row>
@@ -72916,16 +72916,16 @@
         <v>78</v>
       </c>
       <c r="C38" s="25">
-        <v>7.6700000000000004E-2</v>
+        <v>7.8399999999999997E-2</v>
       </c>
       <c r="D38" s="25">
-        <v>8.4900000000000003E-2</v>
+        <v>6.9699999999999998E-2</v>
       </c>
       <c r="E38" s="15">
-        <v>1.81</v>
+        <v>1</v>
       </c>
       <c r="F38" s="15">
-        <v>9.0500000000000007</v>
+        <v>9.44</v>
       </c>
       <c r="G38" s="15">
         <v>71.599999999999994</v>
@@ -72936,16 +72936,16 @@
         <v>81</v>
       </c>
       <c r="C39" s="24">
-        <v>7.0800000000000002E-2</v>
+        <v>6.2399999999999997E-2</v>
       </c>
       <c r="D39" s="24">
-        <v>7.9699999999999993E-2</v>
+        <v>7.1800000000000003E-2</v>
       </c>
       <c r="E39" s="13">
-        <v>1.26</v>
+        <v>0.23</v>
       </c>
       <c r="F39" s="13">
-        <v>9.4</v>
+        <v>10.210000000000001</v>
       </c>
       <c r="G39" s="13">
         <v>77.599999999999994</v>
@@ -72967,6 +72967,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="9973b7cd-78b1-41ec-8b66-6143e90e5574" xsi:nil="true"/>
@@ -72976,15 +72985,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -73249,20 +73249,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95870B3D-2286-404C-93FA-2858F75312B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E8657E7-8F72-4E89-9411-E42EF9EA66A0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="9973b7cd-78b1-41ec-8b66-6143e90e5574"/>
     <ds:schemaRef ds:uri="3b9b9037-28f8-4200-a961-13fb81bc61ed"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95870B3D-2286-404C-93FA-2858F75312B2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>